<commit_message>
Complete the exctract Acitvity data sequence
</commit_message>
<xml_diff>
--- a/Data/Activities Data.xlsx
+++ b/Data/Activities Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <x:si>
     <x:t>Date</x:t>
   </x:si>
@@ -37,64 +37,16 @@
     <x:t>Distance</x:t>
   </x:si>
   <x:si>
-    <x:t>Mon 23 Oct</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2,757</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10,216</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8.12</x:t>
-  </x:si>
-  <x:si>
     <x:t>Tue 24 Oct</x:t>
   </x:si>
   <x:si>
-    <x:t>3,113</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10,983</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8.84</x:t>
-  </x:si>
-  <x:si>
     <x:t>Wed 25 Oct</x:t>
   </x:si>
   <x:si>
-    <x:t>2,863</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13,708</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10.88</x:t>
+    <x:t>Thu 26 Oct</x:t>
   </x:si>
   <x:si>
     <x:t>Today</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1,677</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5,420</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.6</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -451,68 +403,68 @@
       <x:c r="A2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
+      <x:c r="B2" s="0" t="n">
+        <x:v>3113</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>10983</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="n">
+        <x:v>8.84</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
+        <x:v>2863</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>13708</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="n">
+        <x:v>10.88</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>2858</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>10185</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="n">
         <x:v>19</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="n">
+        <x:v>8.28</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="n">
+        <x:v>569</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="n">
+        <x:v>0.05</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Tidy up the code
</commit_message>
<xml_diff>
--- a/Data/Activities Data.xlsx
+++ b/Data/Activities Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Date</x:t>
   </x:si>
@@ -35,6 +35,18 @@
   </x:si>
   <x:si>
     <x:t>Distance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fri 20 Oct</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sat 21 Oct</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sun 22 Oct</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mon 23 Oct</x:t>
   </x:si>
   <x:si>
     <x:t>Tue 24 Oct</x:t>
@@ -404,16 +416,16 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B2" s="0" t="n">
-        <x:v>3113</x:v>
+        <x:v>3257</x:v>
       </x:c>
       <x:c r="C2" s="0" t="n">
-        <x:v>10983</x:v>
+        <x:v>13531</x:v>
       </x:c>
       <x:c r="D2" s="0" t="n">
-        <x:v>13</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E2" s="0" t="n">
-        <x:v>8.84</x:v>
+        <x:v>10.73</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
@@ -421,16 +433,16 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="0" t="n">
-        <x:v>2863</x:v>
+        <x:v>3167</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>13708</x:v>
+        <x:v>15717</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>10.88</x:v>
+        <x:v>11.79</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
@@ -438,16 +450,16 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
-        <x:v>2858</x:v>
+        <x:v>3224</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>10185</x:v>
+        <x:v>14589</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
-        <x:v>19</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>8.28</x:v>
+        <x:v>10.73</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
@@ -455,15 +467,83 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="n">
-        <x:v>569</x:v>
+        <x:v>2757</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
+        <x:v>10216</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="n">
+        <x:v>8.12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="n">
+        <x:v>3113</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>10983</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="n">
+        <x:v>8.84</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="n">
+        <x:v>2863</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="n">
+        <x:v>13708</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="n">
+        <x:v>10.88</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5">
+      <x:c r="A8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="n">
+        <x:v>2858</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
+        <x:v>10185</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="n">
+        <x:v>8.28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="A9" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="n">
+        <x:v>588</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="n">
+      <x:c r="D9" s="0" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="E5" s="0" t="n">
+      <x:c r="E9" s="0" t="n">
         <x:v>0.05</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Complete Read Acvitities Data process. Create Read Sleep Statistics process
</commit_message>
<xml_diff>
--- a/Data/Activities Data.xlsx
+++ b/Data/Activities Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kodowanie\UIPath\fitbit_data_xtractor\fitbit-data-xtractor\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9FEB63-B6CA-4D3C-84DF-96A2E1D894CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD25EE1D-082D-46A0-A9C2-E5C9EB60E15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="23460" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8250" yWindow="1755" windowWidth="19470" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6936,12 +6936,13 @@
   <dimension ref="A1:E2356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>